<commit_message>
Pushing latest changes to repro
</commit_message>
<xml_diff>
--- a/Uploads/Scrappers.xlsx
+++ b/Uploads/Scrappers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-rkammili\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6C3220-A957-4903-B04E-47476777E340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E241E0-9B77-4562-85BA-9F2AEC4887D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
   <si>
-    <t>https://www.microsoft.com/en-us/store/collections/surfaceproaccessories</t>
+    <t>https://www.microsoft.com/en-us/surface</t>
   </si>
 </sst>
 </file>
@@ -356,9 +356,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -371,9 +373,20 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{559D0619-5363-4A9C-8172-347703F7092D}"/>
+    <hyperlink ref="A2:A3" r:id="rId2" display="https://www.microsoft.com/en-us/surface" xr:uid="{6ABAA669-EB38-4314-A73A-8B8FDAC7F635}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Pushing the latest code updates
</commit_message>
<xml_diff>
--- a/Uploads/Scrappers.xlsx
+++ b/Uploads/Scrappers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-rkammili\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E241E0-9B77-4562-85BA-9F2AEC4887D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED4BFC7-FCDD-4F09-9A4F-215307CC60BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,27 +25,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>https://www.microsoft.com/en-us/surface</t>
   </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/surface/devices/surface-pro</t>
+  </si>
+  <si>
+    <t>https://www.microsoft.com/en-us/surface/devices/surface-laptop</t>
+  </si>
+  <si>
+    <t>microsoft.com/en-us/surface/devices/compare-devices</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -68,16 +69,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -356,37 +354,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="90.33203125" customWidth="1"/>
+    <col min="1" max="1" width="64.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{559D0619-5363-4A9C-8172-347703F7092D}"/>
-    <hyperlink ref="A2:A3" r:id="rId2" display="https://www.microsoft.com/en-us/surface" xr:uid="{6ABAA669-EB38-4314-A73A-8B8FDAC7F635}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>